<commit_message>
Sequential abalone debugged; working successfully
</commit_message>
<xml_diff>
--- a/assignment2/results/O2sheet.xlsx
+++ b/assignment2/results/O2sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\diogenes\Efficient_lab\assignment2\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\durga\Desktop\Efficient_lab_report\Profiling\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E58303D-D503-4B08-A8D8-297E9B2F93DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBC97C8-4357-4EC9-B40F-34D0AC427F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="O2" sheetId="1" r:id="rId1"/>
@@ -417,22 +417,22 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,15 +461,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>200</v>
       </c>
       <c r="B2">
-        <v>0.19</v>
+        <v>2.87</v>
       </c>
       <c r="C2" s="2">
-        <v>2.1609839999999999E-4</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="D2" s="2">
         <v>394778</v>
@@ -487,15 +487,15 @@
         <v>2294.5374999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1200</v>
       </c>
       <c r="B3">
-        <v>2.5299999999999998</v>
+        <v>7.79</v>
       </c>
       <c r="C3" s="2">
-        <v>4.0594020000000001E-3</v>
+        <v>0.82</v>
       </c>
       <c r="D3" s="2">
         <v>181508100</v>
@@ -513,15 +513,15 @@
         <v>2294.5614999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2200</v>
       </c>
       <c r="B4">
-        <v>2.74</v>
+        <v>7.83</v>
       </c>
       <c r="C4">
-        <v>0.41</v>
+        <v>81.42</v>
       </c>
       <c r="D4">
         <v>658031900</v>
@@ -539,15 +539,15 @@
         <v>2294.5711999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3200</v>
       </c>
       <c r="B5">
-        <v>2.57</v>
+        <v>7.52</v>
       </c>
       <c r="C5">
-        <v>0.47</v>
+        <v>88.42</v>
       </c>
       <c r="D5">
         <v>1304569000</v>
@@ -565,15 +565,15 @@
         <v>2294.5747999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4200</v>
       </c>
       <c r="B6">
-        <v>2.67</v>
+        <v>7.76</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>86.93</v>
       </c>
       <c r="D6">
         <v>2333585000</v>

</xml_diff>